<commit_message>
removed old landing page
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>YES</t>
-  </si>
-  <si>
-    <t>YES - to be impoved</t>
   </si>
   <si>
     <t>YES
@@ -225,18 +222,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -282,10 +273,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8" hidden="1"/>
@@ -644,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1015,8 +1006,8 @@
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>48</v>
+      <c r="D37" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,8 +1130,8 @@
       <c r="B50">
         <v>1</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>49</v>
+      <c r="D50" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>